<commit_message>
Auto detect xlsx modification, add caseNum to result file, add rng seed
</commit_message>
<xml_diff>
--- a/config/case_list.xlsx
+++ b/config/case_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\svn\file_manage_svn\code\matlab\06_systems\01_ofdmIoT_USRP\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC64C096-C18E-4808-9EC9-D189D08CE220}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8CC66C92-2446-4737-8A34-5A9F9DE013C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" xr2:uid="{0B681031-E668-4EA4-ABFE-801D536798FB}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.5"/>
@@ -596,7 +596,7 @@
         <v>0.25</v>
       </c>
       <c r="I4" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>

</xml_diff>